<commit_message>
theme inf version 1.3
</commit_message>
<xml_diff>
--- a/doc/ThemeInterface.xlsx
+++ b/doc/ThemeInterface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="9630" windowHeight="3540"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="9630" windowHeight="3540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="版本更新历史" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="106">
   <si>
     <t xml:space="preserve">
 </t>
@@ -247,10 +247,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>id:壁纸Id；title:标题；categoryid:壁纸所属分类；subcategoryid:所属子分类；publishtime:发布时间；rating:星级；thumbnail:缩略图地址；downloadnumber:下载次数；ordernumber:排序号；originalurl:原图地址；status:状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://theme.oo523.com/wallpaper/WallPaperdetail?imsi=1111&amp;format=json&amp;id=1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -303,19 +299,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"result":0,"desc":"成功","count":4,"data":[{"id":1,"title":"杭州西湖","categoryid":1,"subcategoryid":1,"publishtime":"2014-01-02 18:06:04","rating":1,"thumbnailurl":"","downloadnumber":1000,"ordernumber":12,"originalurl":"","status":1},{"id":2,"title":"安徽黄山","categoryid":1,"subcategoryid":2,"publishtime":"2014-01-02 18:06:04","rating":1,"thumbnailurl":"","downloadnumber":100,"ordernumber":15,"originalurl":"","status":1},{"id":3,"title":"进击的巨人","categoryid":2,"subcategoryid":3,"publishtime":"2014-01-02 18:06:04","rating":3,"thumbnailurl":"","downloadnumber":100,"ordernumber":20,"originalurl":"","status":1},{"id":4,"title":"哆啦A梦","categoryid":2,"subcategoryid":3,"publishtime":"2014-01-02 18:06:04","rating":3,"thumbnailurl":"","downloadnumber":100,"ordernumber":2,"originalurl":"","status":0}]}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://theme.oo523.com/wallpaper/wallpaperlist?imsi=1111&amp;format=json&amp;categoryid=1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>http://theme.oo523.com/wallpaper/wallpaperlist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id:壁纸Id；title:标题；categoryid:壁纸所属分类；subcategoryid:所属子分类；publishtime:发布时间；rating:星级；thumbnail:缩略图地址；downloadnumber:下载次数；ordernumber:排序号；originalurl:原图地址；status:状态</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -360,10 +348,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>id:类别Id；Name:类别名称；logourl:专题图标；ordernumber:排序号；status:状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://theme.oo523.com/wallpaper/topiclist?imsi=1111&amp;format=json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -422,11 +406,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">{"result":0,"desc":"成功","count":4,"sver":1,"data":[{"id":1,"name":"新年快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p1.jpg","ordernumber":1,"status":1},{"id":2,"name":"元旦快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p2.jpg","ordernumber":2,"status":1},{"id":2,"name":"元旦快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p2.jpg","ordernumber":2,"status":1},{"id":1,"name":"新年快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p1.jpg","ordernumber":1,"status":1}]}
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>V1.2</t>
   </si>
   <si>
@@ -436,6 +415,42 @@
   <si>
     <t xml:space="preserve">增加配置表版本
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.3</t>
+  </si>
+  <si>
+    <t>2014.01.17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id:类别Id；Name:类别名称；logourl:专题图标；summary: 专题;ordernumber:排序号；status:状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{"result":0,"desc":"成功","count":4,"sver":1,"data":[{"id":1,"name":"新年快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p1.jpg","summary":"这一季，有我最深的思念。就让风捎去满心的祝福，缀满你甜蜜的梦境，祝你拥有一个更加灿烂更加辉煌的来年。把美好的祝福，输在这条短信里，信不长情意重，我的好友愿你新年快乐！","ordernumber":1,"status":1},{"id":2,"name":"元旦快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p2.jpg","summary":"这一季，有我最深的思念。就让风捎去满心的祝福，缀满你甜蜜的梦境，祝你拥有一个更加灿烂更加辉煌的来年。把美好的祝福，输在这条短信里，信不长情意重，我的好友愿你新年快乐！","ordernumber":2,"status":1},{"id":2,"name":"元旦快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p2.jpg","summary":"这一季，有我最深的思念。就让风捎去满心的祝福，缀满你甜蜜的梦境，祝你拥有一个更加灿烂更加辉煌的来年。把美好的祝福，输在这条短信里，信不长情意重，我的好友愿你新年快乐！","ordernumber":2,"status":1},{"id":1,"name":"新年快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p1.jpg","summary":"这一季，有我最深的思念。就让风捎去满心的祝福，缀满你甜蜜的梦境，祝你拥有一个更加灿烂更加辉煌的来年。把美好的祝福，输在这条短信里，信不长情意重，我的好友愿你新年快乐！","ordernumber":1,"status":1}]}
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1,增加专题说明字段summary
+2,更正壁纸返回字段
+3,修正现网图片上传
+4,修正壁纸列表参数取值
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id:壁纸Id；title:标题;publishtime:发布时间；thumbnailurl:缩略图地址；downloadnumber:下载次数；ordernumber:排序号；originalurl:原图地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"result":0,"desc":"成功","count":4,"data":[{"id":2,"title":"美女01","publishtime":"2014-01-17 15:36:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnail/th05.jpg","downloadnumber":56,"originalurl":"http://theme.kk874.com/ThemeResources/Original/th05.jpg"},{"id":4,"title":"模特02","publishtime":"2014-01-17 03:36:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnail/th07.jpg","downloadnumber":40,"originalurl":"http://theme.kk874.com/ThemeResources/Original/th07.jpg"},{"id":1,"title":"美女01","publishtime":"2014-01-17 19:36:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnail/th04.jpg","downloadnumber":23,"originalurl":"http://theme.kk874.com/ThemeResources/Original/th04.jpg"},{"id":3,"title":"模特01","publishtime":"2014-01-16 20:36:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnail/th06.jpg","downloadnumber":10,"originalurl":"http://theme.kk874.com/ThemeResources/Original/th06.jpg"}]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id:壁纸Id；title:标题；categoryid:壁纸所属分类；subcategoryid:所属子分类；publishtime:发布时间；rating:星级；thumbnail:缩略图地址；downloadnumber:下载次数；ordernumber:排序号；originalurl:原图地址；status:状态</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -716,18 +731,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -740,17 +743,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -760,6 +757,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -772,6 +781,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1076,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1110,7 +1125,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>44</v>
@@ -1118,37 +1133,45 @@
     </row>
     <row r="3" spans="1:4" ht="66" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="82.5" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -1241,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:O50"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81:O81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1570,84 +1593,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
+      <c r="B3" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="B4" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
     </row>
     <row r="5" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
@@ -1659,20 +1682,20 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
@@ -1682,20 +1705,20 @@
       <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
     </row>
     <row r="7" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
@@ -1705,43 +1728,43 @@
       <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
@@ -1753,20 +1776,20 @@
       <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
@@ -1778,20 +1801,20 @@
       <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
     </row>
     <row r="11" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
@@ -1801,20 +1824,20 @@
       <c r="C11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
     </row>
     <row r="12" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
@@ -1824,43 +1847,43 @@
       <c r="C12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="20"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="16"/>
     </row>
     <row r="13" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="16"/>
     </row>
     <row r="14" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
@@ -1872,123 +1895,123 @@
       <c r="C14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
+      <c r="D14" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
     </row>
     <row r="15" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
+      <c r="B15" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
     </row>
     <row r="16" spans="1:15" s="2" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
+      <c r="B16" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
     </row>
     <row r="19" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
     </row>
     <row r="20" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
+      <c r="B20" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
     </row>
     <row r="21" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
+      <c r="B21" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
     </row>
     <row r="22" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
@@ -2000,20 +2023,20 @@
       <c r="C22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
     </row>
     <row r="23" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
@@ -2023,20 +2046,20 @@
       <c r="C23" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
     </row>
     <row r="24" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
@@ -2046,43 +2069,43 @@
       <c r="C24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
     </row>
     <row r="25" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
@@ -2094,20 +2117,20 @@
       <c r="C26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
     </row>
     <row r="27" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
@@ -2119,20 +2142,20 @@
       <c r="C27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
     </row>
     <row r="28" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
@@ -2142,66 +2165,66 @@
       <c r="C28" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
     </row>
     <row r="29" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="20"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="16"/>
     </row>
     <row r="30" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="16"/>
     </row>
     <row r="31" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
@@ -2213,125 +2236,125 @@
       <c r="C31" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
+      <c r="D31" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
     </row>
     <row r="32" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
+      <c r="B32" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
     </row>
     <row r="33" spans="1:15" s="2" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
+      <c r="B33" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
     </row>
     <row r="34" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15"/>
     <row r="35" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15"/>
     <row r="36" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
+      <c r="A36" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
     </row>
     <row r="37" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
+      <c r="B37" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
     </row>
     <row r="38" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
-      <c r="O38" s="16"/>
+      <c r="B38" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
     </row>
     <row r="39" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
@@ -2343,20 +2366,20 @@
       <c r="C39" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
     </row>
     <row r="40" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
@@ -2366,20 +2389,20 @@
       <c r="C40" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
     </row>
     <row r="41" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
@@ -2389,43 +2412,43 @@
       <c r="C41" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
     </row>
     <row r="42" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="16"/>
     </row>
     <row r="43" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
@@ -2437,20 +2460,20 @@
       <c r="C43" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
     </row>
     <row r="44" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
@@ -2462,20 +2485,20 @@
       <c r="C44" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
     </row>
     <row r="45" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
@@ -2485,20 +2508,20 @@
       <c r="C45" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
     </row>
     <row r="46" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
@@ -2508,43 +2531,43 @@
       <c r="C46" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="20"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="16"/>
     </row>
     <row r="47" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
-      <c r="O47" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="16"/>
     </row>
     <row r="48" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
@@ -2556,62 +2579,62 @@
       <c r="C48" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
+      <c r="D48" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
     </row>
     <row r="49" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="16"/>
-      <c r="M49" s="16"/>
-      <c r="N49" s="16"/>
-      <c r="O49" s="16"/>
-    </row>
-    <row r="50" spans="1:15" s="2" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+    </row>
+    <row r="50" spans="1:15" s="2" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="21"/>
-      <c r="O50" s="21"/>
+      <c r="B50" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
     </row>
     <row r="51" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
@@ -2631,65 +2654,65 @@
       <c r="O51" s="1"/>
     </row>
     <row r="52" spans="1:15" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
     </row>
     <row r="53" spans="1:15" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
+      <c r="B53" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
     </row>
     <row r="54" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="16"/>
-      <c r="J54" s="16"/>
-      <c r="K54" s="16"/>
-      <c r="L54" s="16"/>
-      <c r="M54" s="16"/>
-      <c r="N54" s="16"/>
-      <c r="O54" s="16"/>
+      <c r="B54" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="23"/>
+      <c r="K54" s="23"/>
+      <c r="L54" s="23"/>
+      <c r="M54" s="23"/>
+      <c r="N54" s="23"/>
+      <c r="O54" s="23"/>
     </row>
     <row r="55" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A55" s="5" t="s">
@@ -2701,20 +2724,20 @@
       <c r="C55" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
     </row>
     <row r="56" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A56" s="3"/>
@@ -2724,114 +2747,114 @@
       <c r="C56" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="15"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="15"/>
-      <c r="O56" s="15"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="19"/>
+      <c r="O56" s="19"/>
     </row>
     <row r="57" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3"/>
       <c r="B57" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="15"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
+        <v>66</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="19"/>
+      <c r="O57" s="19"/>
     </row>
     <row r="58" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
+      <c r="D58" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="19"/>
+      <c r="N58" s="19"/>
+      <c r="O58" s="19"/>
     </row>
     <row r="59" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="3"/>
       <c r="B59" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="19"/>
-      <c r="M59" s="19"/>
-      <c r="N59" s="19"/>
-      <c r="O59" s="20"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="16"/>
     </row>
     <row r="60" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3"/>
       <c r="B60" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
-      <c r="M60" s="19"/>
-      <c r="N60" s="19"/>
-      <c r="O60" s="20"/>
+        <v>82</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="16"/>
     </row>
     <row r="61" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
@@ -2841,20 +2864,20 @@
       <c r="C61" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="15"/>
-      <c r="I61" s="15"/>
-      <c r="J61" s="15"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="15"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="19"/>
+      <c r="O61" s="19"/>
     </row>
     <row r="62" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
@@ -2866,20 +2889,20 @@
       <c r="C62" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-      <c r="K62" s="17"/>
-      <c r="L62" s="17"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
     </row>
     <row r="63" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
@@ -2891,20 +2914,20 @@
       <c r="C63" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
-      <c r="K63" s="15"/>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="15"/>
-      <c r="O63" s="15"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="19"/>
     </row>
     <row r="64" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="3"/>
@@ -2914,45 +2937,45 @@
       <c r="C64" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="15"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+      <c r="L64" s="19"/>
+      <c r="M64" s="19"/>
+      <c r="N64" s="19"/>
+      <c r="O64" s="19"/>
     </row>
     <row r="65" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="3"/>
       <c r="B65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="D65" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D65" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="19"/>
-      <c r="M65" s="19"/>
-      <c r="N65" s="19"/>
-      <c r="O65" s="20"/>
-    </row>
-    <row r="66" spans="1:15" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="16"/>
+    </row>
+    <row r="66" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
         <v>0</v>
       </c>
@@ -2962,62 +2985,62 @@
       <c r="C66" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D66" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
-      <c r="I66" s="27"/>
-      <c r="J66" s="27"/>
-      <c r="K66" s="27"/>
-      <c r="L66" s="27"/>
-      <c r="M66" s="27"/>
-      <c r="N66" s="27"/>
-      <c r="O66" s="28"/>
+      <c r="D66" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="21"/>
+      <c r="N66" s="21"/>
+      <c r="O66" s="22"/>
     </row>
     <row r="67" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="16"/>
-      <c r="K67" s="16"/>
-      <c r="L67" s="16"/>
-      <c r="M67" s="16"/>
-      <c r="N67" s="16"/>
-      <c r="O67" s="16"/>
-    </row>
-    <row r="68" spans="1:15" ht="105" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B67" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="23"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
+      <c r="K67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="23"/>
+      <c r="N67" s="23"/>
+      <c r="O67" s="23"/>
+    </row>
+    <row r="68" spans="1:15" ht="154.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
-      <c r="H68" s="21"/>
-      <c r="I68" s="21"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="21"/>
-      <c r="L68" s="21"/>
-      <c r="M68" s="21"/>
-      <c r="N68" s="21"/>
-      <c r="O68" s="21"/>
+      <c r="B68" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+      <c r="J68" s="17"/>
+      <c r="K68" s="17"/>
+      <c r="L68" s="17"/>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
     </row>
     <row r="69" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A69" s="1"/>
@@ -3054,65 +3077,65 @@
       <c r="O70" s="1"/>
     </row>
     <row r="71" spans="1:15" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="14"/>
-      <c r="N71" s="14"/>
-      <c r="O71" s="14"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
+      <c r="H71" s="26"/>
+      <c r="I71" s="26"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="26"/>
+      <c r="L71" s="26"/>
+      <c r="M71" s="26"/>
+      <c r="N71" s="26"/>
+      <c r="O71" s="26"/>
     </row>
     <row r="72" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="15"/>
-      <c r="K72" s="15"/>
-      <c r="L72" s="15"/>
-      <c r="M72" s="15"/>
-      <c r="N72" s="15"/>
-      <c r="O72" s="15"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="19"/>
+      <c r="K72" s="19"/>
+      <c r="L72" s="19"/>
+      <c r="M72" s="19"/>
+      <c r="N72" s="19"/>
+      <c r="O72" s="19"/>
     </row>
     <row r="73" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-      <c r="K73" s="16"/>
-      <c r="L73" s="16"/>
-      <c r="M73" s="16"/>
-      <c r="N73" s="16"/>
-      <c r="O73" s="16"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="23"/>
+      <c r="N73" s="23"/>
+      <c r="O73" s="23"/>
     </row>
     <row r="74" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="5" t="s">
@@ -3124,20 +3147,20 @@
       <c r="C74" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="17" t="s">
+      <c r="D74" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="17"/>
-      <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
-      <c r="M74" s="17"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="18"/>
+      <c r="M74" s="18"/>
+      <c r="N74" s="18"/>
+      <c r="O74" s="18"/>
     </row>
     <row r="75" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="3"/>
@@ -3147,20 +3170,20 @@
       <c r="C75" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D75" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
-      <c r="H75" s="15"/>
-      <c r="I75" s="15"/>
-      <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
-      <c r="L75" s="15"/>
-      <c r="M75" s="15"/>
-      <c r="N75" s="15"/>
-      <c r="O75" s="15"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="19"/>
+      <c r="O75" s="19"/>
     </row>
     <row r="76" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="3"/>
@@ -3170,20 +3193,20 @@
       <c r="C76" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D76" s="15" t="s">
+      <c r="D76" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E76" s="15"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
-      <c r="H76" s="15"/>
-      <c r="I76" s="15"/>
-      <c r="J76" s="15"/>
-      <c r="K76" s="15"/>
-      <c r="L76" s="15"/>
-      <c r="M76" s="15"/>
-      <c r="N76" s="15"/>
-      <c r="O76" s="15"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
+      <c r="L76" s="19"/>
+      <c r="M76" s="19"/>
+      <c r="N76" s="19"/>
+      <c r="O76" s="19"/>
     </row>
     <row r="77" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="3"/>
@@ -3193,20 +3216,20 @@
       <c r="C77" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D77" s="15" t="s">
+      <c r="D77" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E77" s="15"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
-      <c r="I77" s="15"/>
-      <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="15"/>
-      <c r="M77" s="15"/>
-      <c r="N77" s="15"/>
-      <c r="O77" s="15"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="19"/>
+      <c r="K77" s="19"/>
+      <c r="L77" s="19"/>
+      <c r="M77" s="19"/>
+      <c r="N77" s="19"/>
+      <c r="O77" s="19"/>
     </row>
     <row r="78" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="5" t="s">
@@ -3218,20 +3241,20 @@
       <c r="C78" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="17" t="s">
+      <c r="D78" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="17"/>
-      <c r="K78" s="17"/>
-      <c r="L78" s="17"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="18"/>
     </row>
     <row r="79" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
@@ -3243,20 +3266,20 @@
       <c r="C79" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="D79" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E79" s="15"/>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
-      <c r="I79" s="15"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="15"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="15"/>
-      <c r="O79" s="15"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+      <c r="K79" s="19"/>
+      <c r="L79" s="19"/>
+      <c r="M79" s="19"/>
+      <c r="N79" s="19"/>
+      <c r="O79" s="19"/>
     </row>
     <row r="80" spans="1:15" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="3"/>
@@ -3266,20 +3289,20 @@
       <c r="C80" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="D80" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
-      <c r="I80" s="15"/>
-      <c r="J80" s="15"/>
-      <c r="K80" s="15"/>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="15"/>
-      <c r="O80" s="15"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
+      <c r="L80" s="19"/>
+      <c r="M80" s="19"/>
+      <c r="N80" s="19"/>
+      <c r="O80" s="19"/>
     </row>
     <row r="81" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
@@ -3291,62 +3314,62 @@
       <c r="C81" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D81" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
-      <c r="J81" s="27"/>
-      <c r="K81" s="27"/>
-      <c r="L81" s="27"/>
-      <c r="M81" s="27"/>
-      <c r="N81" s="27"/>
-      <c r="O81" s="28"/>
+      <c r="D81" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
+      <c r="J81" s="21"/>
+      <c r="K81" s="21"/>
+      <c r="L81" s="21"/>
+      <c r="M81" s="21"/>
+      <c r="N81" s="21"/>
+      <c r="O81" s="22"/>
     </row>
     <row r="82" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A82" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C82" s="16"/>
-      <c r="D82" s="16"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="16"/>
-      <c r="I82" s="16"/>
-      <c r="J82" s="16"/>
-      <c r="K82" s="16"/>
-      <c r="L82" s="16"/>
-      <c r="M82" s="16"/>
-      <c r="N82" s="16"/>
-      <c r="O82" s="16"/>
+      <c r="B82" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="23"/>
+      <c r="J82" s="23"/>
+      <c r="K82" s="23"/>
+      <c r="L82" s="23"/>
+      <c r="M82" s="23"/>
+      <c r="N82" s="23"/>
+      <c r="O82" s="23"/>
     </row>
     <row r="83" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="21" t="s">
+      <c r="B83" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
-      <c r="E83" s="21"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
-      <c r="H83" s="21"/>
-      <c r="I83" s="21"/>
-      <c r="J83" s="21"/>
-      <c r="K83" s="21"/>
-      <c r="L83" s="21"/>
-      <c r="M83" s="21"/>
-      <c r="N83" s="21"/>
-      <c r="O83" s="21"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
+      <c r="J83" s="17"/>
+      <c r="K83" s="17"/>
+      <c r="L83" s="17"/>
+      <c r="M83" s="17"/>
+      <c r="N83" s="17"/>
+      <c r="O83" s="17"/>
     </row>
     <row r="86" spans="1:15" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A86" s="8" t="s">
@@ -3358,46 +3381,46 @@
       <c r="A87" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B87" s="24" t="s">
+      <c r="B87" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C87" s="25"/>
+      <c r="C87" s="32"/>
     </row>
     <row r="88" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A88" s="11">
         <v>0</v>
       </c>
-      <c r="B88" s="22" t="s">
+      <c r="B88" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C88" s="23"/>
+      <c r="C88" s="25"/>
     </row>
     <row r="89" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A89" s="11">
         <v>997</v>
       </c>
-      <c r="B89" s="22" t="s">
+      <c r="B89" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C89" s="23"/>
+      <c r="C89" s="25"/>
     </row>
     <row r="90" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A90" s="11">
         <v>999</v>
       </c>
-      <c r="B90" s="22" t="s">
+      <c r="B90" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C90" s="23"/>
+      <c r="C90" s="25"/>
     </row>
     <row r="91" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A91" s="11">
         <v>993</v>
       </c>
-      <c r="B91" s="22" t="s">
+      <c r="B91" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C91" s="23"/>
+      <c r="C91" s="25"/>
     </row>
     <row r="96" spans="1:15" ht="186" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="99" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3955,6 +3978,71 @@
     </row>
   </sheetData>
   <mergeCells count="81">
+    <mergeCell ref="D39:O39"/>
+    <mergeCell ref="D40:O40"/>
+    <mergeCell ref="D59:O59"/>
+    <mergeCell ref="D60:O60"/>
+    <mergeCell ref="D41:O41"/>
+    <mergeCell ref="D43:O43"/>
+    <mergeCell ref="D44:O44"/>
+    <mergeCell ref="D45:O45"/>
+    <mergeCell ref="D46:O46"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D61:O61"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B67:O67"/>
+    <mergeCell ref="B68:O68"/>
+    <mergeCell ref="D62:O62"/>
+    <mergeCell ref="D63:O63"/>
+    <mergeCell ref="D64:O64"/>
+    <mergeCell ref="D66:O66"/>
+    <mergeCell ref="D65:O65"/>
+    <mergeCell ref="A71:O71"/>
+    <mergeCell ref="B72:O72"/>
+    <mergeCell ref="B73:O73"/>
+    <mergeCell ref="D74:O74"/>
+    <mergeCell ref="B53:O53"/>
+    <mergeCell ref="D27:O27"/>
+    <mergeCell ref="D28:O28"/>
+    <mergeCell ref="B21:O21"/>
+    <mergeCell ref="D22:O22"/>
+    <mergeCell ref="D23:O23"/>
+    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="B32:O32"/>
+    <mergeCell ref="B33:O33"/>
+    <mergeCell ref="A52:O52"/>
+    <mergeCell ref="D48:O48"/>
+    <mergeCell ref="B49:O49"/>
+    <mergeCell ref="B50:O50"/>
+    <mergeCell ref="A36:O36"/>
+    <mergeCell ref="B37:O37"/>
+    <mergeCell ref="B38:O38"/>
+    <mergeCell ref="D24:O24"/>
+    <mergeCell ref="D26:O26"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B20:O20"/>
+    <mergeCell ref="D12:O12"/>
+    <mergeCell ref="D8:O8"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="D75:O75"/>
+    <mergeCell ref="D76:O76"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="B4:O4"/>
+    <mergeCell ref="D5:O5"/>
+    <mergeCell ref="D6:O6"/>
+    <mergeCell ref="B54:O54"/>
+    <mergeCell ref="D7:O7"/>
+    <mergeCell ref="D9:O9"/>
+    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="D11:O11"/>
+    <mergeCell ref="D14:O14"/>
+    <mergeCell ref="B15:O15"/>
+    <mergeCell ref="B16:O16"/>
+    <mergeCell ref="A19:O19"/>
     <mergeCell ref="D25:O25"/>
     <mergeCell ref="D30:O30"/>
     <mergeCell ref="D42:O42"/>
@@ -3971,71 +4059,6 @@
     <mergeCell ref="D57:O57"/>
     <mergeCell ref="D55:O55"/>
     <mergeCell ref="D56:O56"/>
-    <mergeCell ref="D75:O75"/>
-    <mergeCell ref="D76:O76"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="B4:O4"/>
-    <mergeCell ref="D5:O5"/>
-    <mergeCell ref="D6:O6"/>
-    <mergeCell ref="B54:O54"/>
-    <mergeCell ref="D7:O7"/>
-    <mergeCell ref="D9:O9"/>
-    <mergeCell ref="D10:O10"/>
-    <mergeCell ref="D11:O11"/>
-    <mergeCell ref="D14:O14"/>
-    <mergeCell ref="B15:O15"/>
-    <mergeCell ref="B16:O16"/>
-    <mergeCell ref="A19:O19"/>
-    <mergeCell ref="D24:O24"/>
-    <mergeCell ref="D26:O26"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B20:O20"/>
-    <mergeCell ref="B53:O53"/>
-    <mergeCell ref="D27:O27"/>
-    <mergeCell ref="D28:O28"/>
-    <mergeCell ref="B21:O21"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="D23:O23"/>
-    <mergeCell ref="D31:O31"/>
-    <mergeCell ref="B32:O32"/>
-    <mergeCell ref="B33:O33"/>
-    <mergeCell ref="A52:O52"/>
-    <mergeCell ref="D12:O12"/>
-    <mergeCell ref="D8:O8"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D61:O61"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B67:O67"/>
-    <mergeCell ref="B68:O68"/>
-    <mergeCell ref="D62:O62"/>
-    <mergeCell ref="D63:O63"/>
-    <mergeCell ref="D64:O64"/>
-    <mergeCell ref="D66:O66"/>
-    <mergeCell ref="D65:O65"/>
-    <mergeCell ref="A71:O71"/>
-    <mergeCell ref="B72:O72"/>
-    <mergeCell ref="B73:O73"/>
-    <mergeCell ref="D74:O74"/>
-    <mergeCell ref="D48:O48"/>
-    <mergeCell ref="B49:O49"/>
-    <mergeCell ref="B50:O50"/>
-    <mergeCell ref="D59:O59"/>
-    <mergeCell ref="D60:O60"/>
-    <mergeCell ref="D41:O41"/>
-    <mergeCell ref="D43:O43"/>
-    <mergeCell ref="D44:O44"/>
-    <mergeCell ref="D45:O45"/>
-    <mergeCell ref="D46:O46"/>
-    <mergeCell ref="A36:O36"/>
-    <mergeCell ref="B37:O37"/>
-    <mergeCell ref="B38:O38"/>
-    <mergeCell ref="D39:O39"/>
-    <mergeCell ref="D40:O40"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
modify theme interface doc
</commit_message>
<xml_diff>
--- a/doc/ThemeInterface.xlsx
+++ b/doc/ThemeInterface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="9630" windowHeight="3540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="9630" windowHeight="3540"/>
   </bookViews>
   <sheets>
     <sheet name="版本更新历史" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="132">
   <si>
     <t xml:space="preserve">
 </t>
@@ -296,10 +296,6 @@
   </si>
   <si>
     <t>根据传递的壁纸分类Id或子分类Id获取壁纸列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://theme.oo523.com/wallpaper/wallpaperlist?imsi=1111&amp;format=json&amp;categoryid=1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -396,11 +392,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">{"result":0,"desc":"成功","count":2,"sver":1,"data":[{"id":1,"name":"美女","logourl":"http://theme.kk874.com/ThemeResources/Thumbnail/th1123.jpg","ordernumber":1,"status":1},{"id":2,"name":"动漫","logourl":"http://theme.kk874.com/ThemeResources/Thumbnail/th1111.jpg","ordernumber":2,"status":1}]}
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">{"result":0,"desc":"成功","count":3,"sver":1,"data":[{"categoryid":1,"id":1,"name":"美女之家","logourl":"http://theme.kk874.com/ThemeResources/Thumbnail/th1123.jpg","ordernumber":1,"status":1},{"categoryid":1,"id":2,"name":"模特","logourl":"http://theme.kk874.com/ThemeResources/Thumbnail/th1124.jpg","ordernumber":3,"status":1},{"categoryid":2,"id":3,"name":"动漫1","logourl":"http://theme.kk874.com/ThemeResources/Thumbnail/th1112.jpg","ordernumber":2,"status":1}]}
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -426,11 +417,6 @@
   </si>
   <si>
     <t>id:类别Id；Name:类别名称；logourl:专题图标；summary: 专题;ordernumber:排序号；status:状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{"result":0,"desc":"成功","count":4,"sver":1,"data":[{"id":1,"name":"新年快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p1.jpg","summary":"这一季，有我最深的思念。就让风捎去满心的祝福，缀满你甜蜜的梦境，祝你拥有一个更加灿烂更加辉煌的来年。把美好的祝福，输在这条短信里，信不长情意重，我的好友愿你新年快乐！","ordernumber":1,"status":1},{"id":2,"name":"元旦快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p2.jpg","summary":"这一季，有我最深的思念。就让风捎去满心的祝福，缀满你甜蜜的梦境，祝你拥有一个更加灿烂更加辉煌的来年。把美好的祝福，输在这条短信里，信不长情意重，我的好友愿你新年快乐！","ordernumber":2,"status":1},{"id":2,"name":"元旦快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p2.jpg","summary":"这一季，有我最深的思念。就让风捎去满心的祝福，缀满你甜蜜的梦境，祝你拥有一个更加灿烂更加辉煌的来年。把美好的祝福，输在这条短信里，信不长情意重，我的好友愿你新年快乐！","ordernumber":2,"status":1},{"id":1,"name":"新年快乐","logourl":"http://theme.kk874.com/ThemeResources/Logo/p1.jpg","summary":"这一季，有我最深的思念。就让风捎去满心的祝福，缀满你甜蜜的梦境，祝你拥有一个更加灿烂更加辉煌的来年。把美好的祝福，输在这条短信里，信不长情意重，我的好友愿你新年快乐！","ordernumber":1,"status":1}]}
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -446,11 +432,142 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"result":0,"desc":"成功","count":4,"data":[{"id":2,"title":"美女01","publishtime":"2014-01-17 15:36:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnail/th05.jpg","downloadnumber":56,"originalurl":"http://theme.kk874.com/ThemeResources/Original/th05.jpg"},{"id":4,"title":"模特02","publishtime":"2014-01-17 03:36:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnail/th07.jpg","downloadnumber":40,"originalurl":"http://theme.kk874.com/ThemeResources/Original/th07.jpg"},{"id":1,"title":"美女01","publishtime":"2014-01-17 19:36:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnail/th04.jpg","downloadnumber":23,"originalurl":"http://theme.kk874.com/ThemeResources/Original/th04.jpg"},{"id":3,"title":"模特01","publishtime":"2014-01-16 20:36:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnail/th06.jpg","downloadnumber":10,"originalurl":"http://theme.kk874.com/ThemeResources/Original/th06.jpg"}]}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id:壁纸Id；title:标题；categoryid:壁纸所属分类；subcategoryid:所属子分类；publishtime:发布时间；rating:星级；thumbnail:缩略图地址；downloadnumber:下载次数；ordernumber:排序号；originalurl:原图地址；status:状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>st</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片属性（窄屏为0 宽屏为1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lcd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分辨率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机品牌koobee 非koobee为pcba</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{"result":0,"desc":"成功","count":6,"sver":6,"data":[{"id":0,"name":"全部","logourl":null,"summary":"","ordernumber":0,"status":1},{"id":1,"name":"城市","logourl":null,"summary":"城市","ordernumber":1,"status":1},{"id":2,"name":"风景","logourl":null,"summary":"风景","ordernumber":2,"status":1},{"id":3,"name":"卡通","logourl":null,"summary":"卡通","ordernumber":3,"status":1},{"id":4,"name":"小清新","logourl":null,"summary":"小清新","ordernumber":4,"status":1},{"id":5,"name":"自然","logourl":null,"summary":"自然","ordernumber":5,"status":1}]}
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{"result":0,"desc":"成功","count":4,"sver":12,"data":[{"id":1,"name":"春天在哪里","logourl":"http://theme.kk874.com/ThemeResources/Logos/da9b6dbf-dc04-4e06-8185-080bda4f598a_.jpg","summary":"春天在哪里","ordernumber":1,"status":1},{"id":2,"name":"自然心情","logourl":"http://theme.kk874.com/ThemeResources/Logos/0f6bfec5-e687-4747-ae3c-6c1a7d159648_.jpg","summary":"自然心情","ordernumber":2,"status":1},{"id":3,"name":"卡通乐园","logourl":"http://theme.kk874.com/ThemeResources/Logos/1a5196d4-89a4-4275-b07b-800b9f731a97_.jpg","summary":"卡通乐园","ordernumber":3,"status":1},{"id":4,"name":"热门排行","logourl":"http://theme.kk874.com/ThemeResources/Logos/e909dc00-3d30-43b9-8b6a-134fc3091ae4_.jpg","summary":"热门排行","ordernumber":4,"status":1}]}
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回总数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回当前页数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://theme.oo523.com/wallpaper/wallpaperlist?imsi=111&amp;mf=koobee&amp;lcd=540x960&amp;format=json&amp;categoryid=0&amp;st=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"result":0,"desc":"成功","count":2,"total":2,"data":[{"id":102,"title":"城市双01","publishtime":"2014-03-21 11:44:55","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnails/1080x960_582d4783-a452-4aac-8195-089ed5e586d2_.jpg","downloadnumber":94,"originalurl":"http://theme.kk874.com/ThemeResources/Originals/1080x960_0b7a664a-6673-404f-8ee0-d903f04fdadb_.jpg"},{"id":103,"title":"城市双02","publishtime":"2014-03-21 11:48:27","thumbnailurl":"http://theme.kk874.com/ThemeResources/Thumbnails/1080x960_87eb4377-bd11-4903-8dda-63a49c1f2304_.jpg","downloadnumber":56,"originalurl":"http://theme.kk874.com/ThemeResources/Originals/1080x960_2c8f328d-11ff-494f-9c0a-69f5ead632b4_.jpg"}]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2014.01.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2014.03.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,修订topiclist字段
+2,wallpaperlist增加total字段
+3,修正图片上传路径
+4,增加wallpaperno唯一标识字段
+5,修订壁纸配置表版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2014.03.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2014.03.19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1,修正现网图片上传，除了同比例显示可压缩处理，其余属性不做处理
+2,修改管理后台缩略图和原图上传尺寸
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2014.03.31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1,增加图片属性screen type字段
+2,区分koobee和pcba品牌过滤
+3,删除wallpaperno字段方便管理，用id 做唯一区分
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1,代码拆分
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1,修正上传宽屏参数匹配图片bug
+2,修改管理后台缩略图和原图上传尺寸
+3,增加缓存锁
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -688,7 +805,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -740,14 +857,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -758,17 +899,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -778,15 +913,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1091,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1125,7 +1251,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>44</v>
@@ -1133,51 +1259,116 @@
     </row>
     <row r="3" spans="1:4" ht="66" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>75</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="82.5" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="82.5" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="66" x14ac:dyDescent="0.15">
+      <c r="A7" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.15">
+      <c r="A8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="66" x14ac:dyDescent="0.15">
+      <c r="A9" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
+      <c r="A10" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
     <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -1262,16 +1453,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q131"/>
+  <dimension ref="A1:Q135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81:O81"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q65" sqref="Q65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="23.375" style="1" customWidth="1"/>
     <col min="5" max="256" width="9" style="1"/>
@@ -1593,84 +1784,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="29"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
     </row>
     <row r="5" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
@@ -1682,20 +1873,20 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
     </row>
     <row r="6" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
@@ -1705,20 +1896,20 @@
       <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
@@ -1728,43 +1919,43 @@
       <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="16"/>
+      <c r="D8" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
     </row>
     <row r="9" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
@@ -1776,20 +1967,20 @@
       <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
@@ -1801,20 +1992,20 @@
       <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
@@ -1824,20 +2015,20 @@
       <c r="C11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
     </row>
     <row r="12" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
@@ -1847,43 +2038,43 @@
       <c r="C12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="16"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="21"/>
     </row>
     <row r="13" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="16"/>
+        <v>88</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="21"/>
     </row>
     <row r="14" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
@@ -1895,123 +2086,123 @@
       <c r="C14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
     </row>
     <row r="15" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-    </row>
-    <row r="16" spans="1:15" s="2" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+    </row>
+    <row r="16" spans="1:15" s="2" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
+      <c r="B16" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
     </row>
     <row r="19" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
     </row>
     <row r="20" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
     </row>
     <row r="21" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
     </row>
     <row r="22" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
@@ -2023,20 +2214,20 @@
       <c r="C22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
     </row>
     <row r="23" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
@@ -2046,20 +2237,20 @@
       <c r="C23" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
     </row>
     <row r="24" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
@@ -2069,43 +2260,43 @@
       <c r="C24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
     </row>
     <row r="25" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="16"/>
+      <c r="D25" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="21"/>
     </row>
     <row r="26" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
@@ -2117,20 +2308,20 @@
       <c r="C26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
     </row>
     <row r="27" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
@@ -2142,20 +2333,20 @@
       <c r="C27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
     </row>
     <row r="28" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
@@ -2165,20 +2356,20 @@
       <c r="C28" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
     </row>
     <row r="29" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
@@ -2188,43 +2379,43 @@
       <c r="C29" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="16"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="21"/>
     </row>
     <row r="30" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="16"/>
+        <v>88</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="21"/>
     </row>
     <row r="31" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
@@ -2236,125 +2427,125 @@
       <c r="C31" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
     </row>
     <row r="32" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
     </row>
     <row r="33" spans="1:15" s="2" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
+      <c r="B33" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="27"/>
     </row>
     <row r="34" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15"/>
     <row r="35" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15"/>
     <row r="36" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
+      <c r="A36" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
     </row>
     <row r="37" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
+      <c r="B37" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
     </row>
     <row r="38" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
+      <c r="B38" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
     </row>
     <row r="39" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
@@ -2366,20 +2557,20 @@
       <c r="C39" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
     </row>
     <row r="40" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
@@ -2389,20 +2580,20 @@
       <c r="C40" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
     </row>
     <row r="41" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
@@ -2412,43 +2603,43 @@
       <c r="C41" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
     </row>
     <row r="42" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="16"/>
+      <c r="D42" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="21"/>
     </row>
     <row r="43" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
@@ -2460,20 +2651,20 @@
       <c r="C43" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
     </row>
     <row r="44" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
@@ -2485,20 +2676,20 @@
       <c r="C44" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
     </row>
     <row r="45" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
@@ -2508,20 +2699,20 @@
       <c r="C45" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
     </row>
     <row r="46" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
@@ -2531,43 +2722,43 @@
       <c r="C46" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D46" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="16"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="20"/>
+      <c r="O46" s="21"/>
     </row>
     <row r="47" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="16"/>
+        <v>88</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="21"/>
     </row>
     <row r="48" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
@@ -2579,62 +2770,62 @@
       <c r="C48" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="19"/>
-      <c r="N48" s="19"/>
-      <c r="O48" s="19"/>
+      <c r="D48" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
     </row>
     <row r="49" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="M49" s="23"/>
-      <c r="N49" s="23"/>
-      <c r="O49" s="23"/>
-    </row>
-    <row r="50" spans="1:15" s="2" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
+    </row>
+    <row r="50" spans="1:15" s="2" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="17"/>
-      <c r="K50" s="17"/>
-      <c r="L50" s="17"/>
-      <c r="M50" s="17"/>
-      <c r="N50" s="17"/>
-      <c r="O50" s="17"/>
+      <c r="B50" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="27"/>
+      <c r="N50" s="27"/>
+      <c r="O50" s="27"/>
     </row>
     <row r="51" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
@@ -2654,65 +2845,65 @@
       <c r="O51" s="1"/>
     </row>
     <row r="52" spans="1:15" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="26"/>
-      <c r="K52" s="26"/>
-      <c r="L52" s="26"/>
-      <c r="M52" s="26"/>
-      <c r="N52" s="26"/>
-      <c r="O52" s="26"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="31"/>
+      <c r="O52" s="31"/>
     </row>
     <row r="53" spans="1:15" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
     </row>
     <row r="54" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="23"/>
-      <c r="L54" s="23"/>
-      <c r="M54" s="23"/>
-      <c r="N54" s="23"/>
-      <c r="O54" s="23"/>
+      <c r="B54" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
     </row>
     <row r="55" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A55" s="5" t="s">
@@ -2724,20 +2915,20 @@
       <c r="C55" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="D55" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-      <c r="N55" s="18"/>
-      <c r="O55" s="18"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
     </row>
     <row r="56" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A56" s="3"/>
@@ -2747,340 +2938,358 @@
       <c r="C56" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D56" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="19"/>
-      <c r="N56" s="19"/>
-      <c r="O56" s="19"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
     </row>
     <row r="57" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3"/>
       <c r="B57" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D57" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="19"/>
-      <c r="M57" s="19"/>
-      <c r="N57" s="19"/>
-      <c r="O57" s="19"/>
+      <c r="D57" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
     </row>
     <row r="58" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="19"/>
-      <c r="O58" s="19"/>
+      <c r="D58" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
     </row>
     <row r="59" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="3"/>
       <c r="B59" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="16"/>
+        <v>81</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="20"/>
+      <c r="N59" s="20"/>
+      <c r="O59" s="21"/>
     </row>
     <row r="60" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3"/>
       <c r="B60" s="6" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="16"/>
+        <v>106</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="21"/>
     </row>
     <row r="61" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
       <c r="B61" s="6" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
-      <c r="M61" s="19"/>
-      <c r="N61" s="19"/>
-      <c r="O61" s="19"/>
+        <v>109</v>
+      </c>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="21"/>
     </row>
     <row r="62" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
-      <c r="M62" s="18"/>
-      <c r="N62" s="18"/>
-      <c r="O62" s="18"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="21"/>
     </row>
     <row r="63" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A63" s="3"/>
       <c r="B63" s="6" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
-      <c r="M63" s="19"/>
-      <c r="N63" s="19"/>
-      <c r="O63" s="19"/>
+        <v>104</v>
+      </c>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="20"/>
+      <c r="M63" s="20"/>
+      <c r="N63" s="20"/>
+      <c r="O63" s="21"/>
     </row>
     <row r="64" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="3"/>
       <c r="B64" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
-      <c r="L64" s="19"/>
-      <c r="M64" s="19"/>
-      <c r="N64" s="19"/>
-      <c r="O64" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
+      <c r="M64" s="18"/>
+      <c r="N64" s="18"/>
+      <c r="O64" s="18"/>
     </row>
     <row r="65" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="3"/>
-      <c r="B65" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="16"/>
-    </row>
-    <row r="66" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A65" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+      <c r="J65" s="17"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+    </row>
+    <row r="66" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B66" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="18"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+    </row>
+    <row r="67" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="3"/>
+      <c r="B67" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="18"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="18"/>
+    </row>
+    <row r="68" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="3"/>
+      <c r="B68" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="20"/>
+      <c r="M68" s="20"/>
+      <c r="N68" s="20"/>
+      <c r="O68" s="21"/>
+    </row>
+    <row r="69" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="3"/>
+      <c r="B69" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="16"/>
+    </row>
+    <row r="70" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A70" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C70" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D66" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
-      <c r="L66" s="21"/>
-      <c r="M66" s="21"/>
-      <c r="N66" s="21"/>
-      <c r="O66" s="22"/>
-    </row>
-    <row r="67" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="4" t="s">
+      <c r="D70" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="29"/>
+      <c r="K70" s="29"/>
+      <c r="L70" s="29"/>
+      <c r="M70" s="29"/>
+      <c r="N70" s="29"/>
+      <c r="O70" s="30"/>
+    </row>
+    <row r="71" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="23"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="23"/>
-    </row>
-    <row r="68" spans="1:15" ht="154.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="17"/>
-      <c r="K68" s="17"/>
-      <c r="L68" s="17"/>
-      <c r="M68" s="17"/>
-      <c r="N68" s="17"/>
-      <c r="O68" s="17"/>
-    </row>
-    <row r="69" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-    </row>
-    <row r="70" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-    </row>
-    <row r="71" spans="1:15" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B71" s="26"/>
+      <c r="B71" s="26" t="s">
+        <v>115</v>
+      </c>
       <c r="C71" s="26"/>
       <c r="D71" s="26"/>
       <c r="E71" s="26"/>
@@ -3095,403 +3304,409 @@
       <c r="N71" s="26"/>
       <c r="O71" s="26"/>
     </row>
-    <row r="72" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B72" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="27"/>
+      <c r="I72" s="27"/>
+      <c r="J72" s="27"/>
+      <c r="K72" s="27"/>
+      <c r="L72" s="27"/>
+      <c r="M72" s="27"/>
+      <c r="N72" s="27"/>
+      <c r="O72" s="27"/>
+    </row>
+    <row r="73" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+    </row>
+    <row r="74" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+    </row>
+    <row r="75" spans="1:15" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="31"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
+      <c r="N75" s="31"/>
+      <c r="O75" s="31"/>
+    </row>
+    <row r="76" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B76" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="19"/>
-      <c r="J72" s="19"/>
-      <c r="K72" s="19"/>
-      <c r="L72" s="19"/>
-      <c r="M72" s="19"/>
-      <c r="N72" s="19"/>
-      <c r="O72" s="19"/>
-    </row>
-    <row r="73" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="4" t="s">
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="18"/>
+      <c r="M76" s="18"/>
+      <c r="N76" s="18"/>
+      <c r="O76" s="18"/>
+    </row>
+    <row r="77" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B73" s="23" t="s">
+      <c r="B77" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="23"/>
-      <c r="J73" s="23"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="23"/>
-      <c r="N73" s="23"/>
-      <c r="O73" s="23"/>
-    </row>
-    <row r="74" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="5" t="s">
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
+      <c r="F77" s="26"/>
+      <c r="G77" s="26"/>
+      <c r="H77" s="26"/>
+      <c r="I77" s="26"/>
+      <c r="J77" s="26"/>
+      <c r="K77" s="26"/>
+      <c r="L77" s="26"/>
+      <c r="M77" s="26"/>
+      <c r="N77" s="26"/>
+      <c r="O77" s="26"/>
+    </row>
+    <row r="78" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-      <c r="L74" s="18"/>
-      <c r="M74" s="18"/>
-      <c r="N74" s="18"/>
-      <c r="O74" s="18"/>
-    </row>
-    <row r="75" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="3"/>
-      <c r="B75" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="19"/>
-      <c r="J75" s="19"/>
-      <c r="K75" s="19"/>
-      <c r="L75" s="19"/>
-      <c r="M75" s="19"/>
-      <c r="N75" s="19"/>
-      <c r="O75" s="19"/>
-    </row>
-    <row r="76" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="3"/>
-      <c r="B76" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E76" s="19"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-      <c r="J76" s="19"/>
-      <c r="K76" s="19"/>
-      <c r="L76" s="19"/>
-      <c r="M76" s="19"/>
-      <c r="N76" s="19"/>
-      <c r="O76" s="19"/>
-    </row>
-    <row r="77" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="3"/>
-      <c r="B77" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E77" s="19"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
-      <c r="J77" s="19"/>
-      <c r="K77" s="19"/>
-      <c r="L77" s="19"/>
-      <c r="M77" s="19"/>
-      <c r="N77" s="19"/>
-      <c r="O77" s="19"/>
-    </row>
-    <row r="78" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D78" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="18"/>
-      <c r="K78" s="18"/>
-      <c r="L78" s="18"/>
-      <c r="M78" s="18"/>
-      <c r="N78" s="18"/>
-      <c r="O78" s="18"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+      <c r="J78" s="17"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
     </row>
     <row r="79" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A79" s="3"/>
       <c r="B79" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E79" s="19"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
-      <c r="J79" s="19"/>
-      <c r="K79" s="19"/>
-      <c r="L79" s="19"/>
-      <c r="M79" s="19"/>
-      <c r="N79" s="19"/>
-      <c r="O79" s="19"/>
-    </row>
-    <row r="80" spans="1:15" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="18"/>
+      <c r="M79" s="18"/>
+      <c r="N79" s="18"/>
+      <c r="O79" s="18"/>
+    </row>
+    <row r="80" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="3"/>
       <c r="B80" s="6" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E80" s="19"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="19"/>
-      <c r="I80" s="19"/>
-      <c r="J80" s="19"/>
-      <c r="K80" s="19"/>
-      <c r="L80" s="19"/>
-      <c r="M80" s="19"/>
-      <c r="N80" s="19"/>
-      <c r="O80" s="19"/>
-    </row>
-    <row r="81" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="18"/>
+      <c r="M80" s="18"/>
+      <c r="N80" s="18"/>
+      <c r="O80" s="18"/>
+    </row>
+    <row r="81" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="3"/>
       <c r="B81" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D81" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="21"/>
-      <c r="H81" s="21"/>
-      <c r="I81" s="21"/>
-      <c r="J81" s="21"/>
-      <c r="K81" s="21"/>
-      <c r="L81" s="21"/>
-      <c r="M81" s="21"/>
-      <c r="N81" s="21"/>
-      <c r="O81" s="22"/>
-    </row>
-    <row r="82" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A82" s="4" t="s">
+      <c r="D81" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+    </row>
+    <row r="82" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
+      <c r="J82" s="17"/>
+      <c r="K82" s="17"/>
+      <c r="L82" s="17"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+    </row>
+    <row r="83" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="18"/>
+      <c r="M83" s="18"/>
+      <c r="N83" s="18"/>
+      <c r="O83" s="18"/>
+    </row>
+    <row r="84" spans="1:15" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="3"/>
+      <c r="B84" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="18"/>
+      <c r="O84" s="18"/>
+    </row>
+    <row r="85" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29"/>
+      <c r="K85" s="29"/>
+      <c r="L85" s="29"/>
+      <c r="M85" s="29"/>
+      <c r="N85" s="29"/>
+      <c r="O85" s="30"/>
+    </row>
+    <row r="86" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A86" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="23" t="s">
+      <c r="B86" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="23"/>
-      <c r="H82" s="23"/>
-      <c r="I82" s="23"/>
-      <c r="J82" s="23"/>
-      <c r="K82" s="23"/>
-      <c r="L82" s="23"/>
-      <c r="M82" s="23"/>
-      <c r="N82" s="23"/>
-      <c r="O82" s="23"/>
-    </row>
-    <row r="83" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="7" t="s">
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="26"/>
+      <c r="J86" s="26"/>
+      <c r="K86" s="26"/>
+      <c r="L86" s="26"/>
+      <c r="M86" s="26"/>
+      <c r="N86" s="26"/>
+      <c r="O86" s="26"/>
+    </row>
+    <row r="87" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B87" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="17"/>
-      <c r="K83" s="17"/>
-      <c r="L83" s="17"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-    </row>
-    <row r="86" spans="1:15" ht="22.5" x14ac:dyDescent="0.15">
-      <c r="A86" s="8" t="s">
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="27"/>
+      <c r="I87" s="27"/>
+      <c r="J87" s="27"/>
+      <c r="K87" s="27"/>
+      <c r="L87" s="27"/>
+      <c r="M87" s="27"/>
+      <c r="N87" s="27"/>
+      <c r="O87" s="27"/>
+    </row>
+    <row r="90" spans="1:15" ht="22.5" x14ac:dyDescent="0.15">
+      <c r="A90" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B86" s="9"/>
-    </row>
-    <row r="87" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A87" s="10" t="s">
+      <c r="B90" s="9"/>
+    </row>
+    <row r="91" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A91" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B87" s="31" t="s">
+      <c r="B91" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C87" s="32"/>
-    </row>
-    <row r="88" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A88" s="11">
+      <c r="C91" s="25"/>
+    </row>
+    <row r="92" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A92" s="11">
         <v>0</v>
       </c>
-      <c r="B88" s="24" t="s">
+      <c r="B92" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C88" s="25"/>
-    </row>
-    <row r="89" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A89" s="11">
+      <c r="C92" s="23"/>
+    </row>
+    <row r="93" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A93" s="11">
         <v>997</v>
       </c>
-      <c r="B89" s="24" t="s">
+      <c r="B93" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C89" s="25"/>
-    </row>
-    <row r="90" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A90" s="11">
+      <c r="C93" s="23"/>
+    </row>
+    <row r="94" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A94" s="11">
         <v>999</v>
       </c>
-      <c r="B90" s="24" t="s">
+      <c r="B94" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C90" s="25"/>
-    </row>
-    <row r="91" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A91" s="11">
+      <c r="C94" s="23"/>
+    </row>
+    <row r="95" spans="1:15" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A95" s="11">
         <v>993</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B95" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C91" s="25"/>
-    </row>
-    <row r="96" spans="1:15" ht="186" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
-      <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
-      <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
-      <c r="O99" s="1"/>
-    </row>
-    <row r="100" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="1"/>
-    </row>
-    <row r="101" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
-    </row>
-    <row r="102" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="1"/>
-    </row>
-    <row r="103" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C95" s="23"/>
+    </row>
+    <row r="100" spans="1:15" ht="186" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" spans="1:15" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3678,7 +3893,7 @@
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
     </row>
-    <row r="114" spans="1:17" s="2" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3712,7 +3927,7 @@
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
     </row>
-    <row r="116" spans="1:17" s="2" customFormat="1" ht="164.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3729,7 +3944,41 @@
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
     </row>
-    <row r="119" spans="1:17" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+      <c r="N117" s="1"/>
+      <c r="O117" s="1"/>
+    </row>
+    <row r="118" spans="1:17" s="2" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+      <c r="N118" s="1"/>
+      <c r="O118" s="1"/>
+    </row>
+    <row r="119" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3745,10 +3994,8 @@
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
       <c r="O119" s="1"/>
-      <c r="P119" s="1"/>
-      <c r="Q119" s="1"/>
-    </row>
-    <row r="120" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="120" spans="1:17" s="2" customFormat="1" ht="164.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3764,48 +4011,8 @@
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
-      <c r="P120" s="1"/>
-      <c r="Q120" s="1"/>
-    </row>
-    <row r="121" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
-      <c r="I121" s="1"/>
-      <c r="J121" s="1"/>
-      <c r="K121" s="1"/>
-      <c r="L121" s="1"/>
-      <c r="M121" s="1"/>
-      <c r="N121" s="1"/>
-      <c r="O121" s="1"/>
-      <c r="P121" s="1"/>
-      <c r="Q121" s="1"/>
-    </row>
-    <row r="122" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-      <c r="F122" s="1"/>
-      <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
-      <c r="I122" s="1"/>
-      <c r="J122" s="1"/>
-      <c r="K122" s="1"/>
-      <c r="L122" s="1"/>
-      <c r="M122" s="1"/>
-      <c r="N122" s="1"/>
-      <c r="O122" s="1"/>
-      <c r="P122" s="1"/>
-      <c r="Q122" s="1"/>
-    </row>
-    <row r="123" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="123" spans="1:17" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3957,7 +4164,7 @@
       <c r="P130" s="1"/>
       <c r="Q130" s="1"/>
     </row>
-    <row r="131" spans="1:17" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3976,60 +4183,103 @@
       <c r="P131" s="1"/>
       <c r="Q131" s="1"/>
     </row>
+    <row r="132" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
+      <c r="O132" s="1"/>
+      <c r="P132" s="1"/>
+      <c r="Q132" s="1"/>
+    </row>
+    <row r="133" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="N133" s="1"/>
+      <c r="O133" s="1"/>
+      <c r="P133" s="1"/>
+      <c r="Q133" s="1"/>
+    </row>
+    <row r="134" spans="1:17" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
+      <c r="O134" s="1"/>
+      <c r="P134" s="1"/>
+      <c r="Q134" s="1"/>
+    </row>
+    <row r="135" spans="1:17" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+      <c r="O135" s="1"/>
+      <c r="P135" s="1"/>
+      <c r="Q135" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="81">
-    <mergeCell ref="D39:O39"/>
-    <mergeCell ref="D40:O40"/>
-    <mergeCell ref="D59:O59"/>
-    <mergeCell ref="D60:O60"/>
-    <mergeCell ref="D41:O41"/>
-    <mergeCell ref="D43:O43"/>
-    <mergeCell ref="D44:O44"/>
-    <mergeCell ref="D45:O45"/>
-    <mergeCell ref="D46:O46"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D61:O61"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B67:O67"/>
-    <mergeCell ref="B68:O68"/>
-    <mergeCell ref="D62:O62"/>
+  <mergeCells count="84">
+    <mergeCell ref="D30:O30"/>
+    <mergeCell ref="D42:O42"/>
+    <mergeCell ref="D47:O47"/>
+    <mergeCell ref="B87:O87"/>
+    <mergeCell ref="D29:O29"/>
+    <mergeCell ref="D82:O82"/>
+    <mergeCell ref="D83:O83"/>
+    <mergeCell ref="D84:O84"/>
+    <mergeCell ref="D85:O85"/>
+    <mergeCell ref="B86:O86"/>
+    <mergeCell ref="D81:O81"/>
+    <mergeCell ref="D58:O58"/>
+    <mergeCell ref="D57:O57"/>
+    <mergeCell ref="D55:O55"/>
+    <mergeCell ref="D56:O56"/>
     <mergeCell ref="D63:O63"/>
-    <mergeCell ref="D64:O64"/>
-    <mergeCell ref="D66:O66"/>
-    <mergeCell ref="D65:O65"/>
-    <mergeCell ref="A71:O71"/>
-    <mergeCell ref="B72:O72"/>
-    <mergeCell ref="B73:O73"/>
-    <mergeCell ref="D74:O74"/>
-    <mergeCell ref="B53:O53"/>
-    <mergeCell ref="D27:O27"/>
-    <mergeCell ref="D28:O28"/>
-    <mergeCell ref="B21:O21"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="D23:O23"/>
-    <mergeCell ref="D31:O31"/>
-    <mergeCell ref="B32:O32"/>
-    <mergeCell ref="B33:O33"/>
-    <mergeCell ref="A52:O52"/>
-    <mergeCell ref="D48:O48"/>
-    <mergeCell ref="B49:O49"/>
-    <mergeCell ref="B50:O50"/>
-    <mergeCell ref="A36:O36"/>
-    <mergeCell ref="B37:O37"/>
-    <mergeCell ref="B38:O38"/>
-    <mergeCell ref="D24:O24"/>
-    <mergeCell ref="D26:O26"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B20:O20"/>
-    <mergeCell ref="D12:O12"/>
-    <mergeCell ref="D8:O8"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="D75:O75"/>
-    <mergeCell ref="D76:O76"/>
-    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="D79:O79"/>
+    <mergeCell ref="D80:O80"/>
+    <mergeCell ref="B95:C95"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="B4:O4"/>
     <mergeCell ref="D5:O5"/>
@@ -4043,22 +4293,58 @@
     <mergeCell ref="B15:O15"/>
     <mergeCell ref="B16:O16"/>
     <mergeCell ref="A19:O19"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B20:O20"/>
+    <mergeCell ref="D12:O12"/>
+    <mergeCell ref="D8:O8"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="B32:O32"/>
+    <mergeCell ref="B33:O33"/>
+    <mergeCell ref="A52:O52"/>
+    <mergeCell ref="D48:O48"/>
+    <mergeCell ref="B49:O49"/>
+    <mergeCell ref="B50:O50"/>
+    <mergeCell ref="A36:O36"/>
+    <mergeCell ref="B37:O37"/>
+    <mergeCell ref="B38:O38"/>
+    <mergeCell ref="D27:O27"/>
+    <mergeCell ref="D28:O28"/>
+    <mergeCell ref="B21:O21"/>
+    <mergeCell ref="D22:O22"/>
+    <mergeCell ref="D23:O23"/>
+    <mergeCell ref="D24:O24"/>
+    <mergeCell ref="D26:O26"/>
     <mergeCell ref="D25:O25"/>
-    <mergeCell ref="D30:O30"/>
-    <mergeCell ref="D42:O42"/>
-    <mergeCell ref="D47:O47"/>
-    <mergeCell ref="B83:O83"/>
-    <mergeCell ref="D29:O29"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D64:O64"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B71:O71"/>
+    <mergeCell ref="B72:O72"/>
+    <mergeCell ref="D65:O65"/>
+    <mergeCell ref="D66:O66"/>
+    <mergeCell ref="D67:O67"/>
+    <mergeCell ref="D70:O70"/>
+    <mergeCell ref="D68:O68"/>
+    <mergeCell ref="A75:O75"/>
+    <mergeCell ref="B76:O76"/>
+    <mergeCell ref="B77:O77"/>
     <mergeCell ref="D78:O78"/>
-    <mergeCell ref="D79:O79"/>
-    <mergeCell ref="D80:O80"/>
-    <mergeCell ref="D81:O81"/>
-    <mergeCell ref="B82:O82"/>
-    <mergeCell ref="D77:O77"/>
-    <mergeCell ref="D58:O58"/>
-    <mergeCell ref="D57:O57"/>
-    <mergeCell ref="D55:O55"/>
-    <mergeCell ref="D56:O56"/>
+    <mergeCell ref="D39:O39"/>
+    <mergeCell ref="D40:O40"/>
+    <mergeCell ref="D59:O59"/>
+    <mergeCell ref="D62:O62"/>
+    <mergeCell ref="D41:O41"/>
+    <mergeCell ref="D43:O43"/>
+    <mergeCell ref="D44:O44"/>
+    <mergeCell ref="D45:O45"/>
+    <mergeCell ref="D46:O46"/>
+    <mergeCell ref="B53:O53"/>
+    <mergeCell ref="D61:O61"/>
+    <mergeCell ref="D60:O60"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4067,9 +4353,9 @@
     <hyperlink ref="B21" r:id="rId3"/>
     <hyperlink ref="B32" r:id="rId4"/>
     <hyperlink ref="B54" r:id="rId5"/>
-    <hyperlink ref="B67" r:id="rId6"/>
-    <hyperlink ref="B73" r:id="rId7"/>
-    <hyperlink ref="B82" r:id="rId8"/>
+    <hyperlink ref="B71" r:id="rId6"/>
+    <hyperlink ref="B77" r:id="rId7"/>
+    <hyperlink ref="B86" r:id="rId8"/>
     <hyperlink ref="B38" r:id="rId9"/>
     <hyperlink ref="B49" r:id="rId10"/>
   </hyperlinks>

</xml_diff>